<commit_message>
added additional columns to the samui output files for xenium samples
</commit_message>
<xml_diff>
--- a/xenium_HYP/raw-data/sample-info/demos_by_sampleid-xen.xlsx
+++ b/xenium_HYP/raw-data/sample-info/demos_by_sampleid-xen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/zk/dyx0glj52sn6_7db_dn0p2vc0000gn/T/ch.sudo.cyberduck/editor-3f24765b-cc4f-4bd7-8256-e435931ba961/dcs04/lieber/marmaypag/spatialHYP_LIBD4195/spatial_HYP/xenium_HYP/raw-data/sample-info/1371818961/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/zk/dyx0glj52sn6_7db_dn0p2vc0000gn/T/ch.sudo.cyberduck/editor-3f24765b-cc4f-4bd7-8256-e435931ba961/dcs04/lieber/marmaypag/spatialHYP_LIBD4195/spatial_HYP/xenium_HYP/raw-data/sample-info/528783301/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1301011F-2647-3E40-96EB-FC1304BACB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8FBC81-1BC6-7C40-A1F0-07DE79332841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31820" yWindow="5800" windowWidth="24440" windowHeight="12940" xr2:uid="{1DB9EFC4-81BF-1747-9C05-D3C9C2D83113}"/>
+    <workbookView xWindow="3900" yWindow="3440" windowWidth="24440" windowHeight="12940" xr2:uid="{1DB9EFC4-81BF-1747-9C05-D3C9C2D83113}"/>
   </bookViews>
   <sheets>
     <sheet name="demos_by_sampleid" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
   <si>
     <t>brnum</t>
   </si>
@@ -134,45 +134,6 @@
     <t>image</t>
   </si>
   <si>
-    <t>X36_5459A__x5459B_M_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X36_5459B__x5459C_M_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X36_8667C__x8667B_F_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X86_reg1__x6197B_M_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X86_reg2__x5993B_F_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X86_reg3__x5993C_F_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X97_reg1__x1735B_M_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X97_reg2__x1735C_M_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X97_reg3__x6588C_F_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X99_1225A__x1225B_M_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X99_1225B__x1225C_M_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X99_8741C__x8741C_F_blackbkgd.png</t>
-  </si>
-  <si>
-    <t>X99_8741D__x8741D_F_domainbounds.png</t>
-  </si>
-  <si>
     <t>output-XETG00089__00011586__Region_1__20231019__161214</t>
   </si>
   <si>
@@ -213,6 +174,87 @@
   </si>
   <si>
     <t>output-XETG00089__0011199__11199X_8741D_HYP__20240223__174831</t>
+  </si>
+  <si>
+    <t>obj_id</t>
+  </si>
+  <si>
+    <t>X36_5459A</t>
+  </si>
+  <si>
+    <t>X36_5459B</t>
+  </si>
+  <si>
+    <t>X36_8667C</t>
+  </si>
+  <si>
+    <t>X86_reg1</t>
+  </si>
+  <si>
+    <t>X86_reg2</t>
+  </si>
+  <si>
+    <t>X86_reg3</t>
+  </si>
+  <si>
+    <t>X97_reg1</t>
+  </si>
+  <si>
+    <t>X97_reg2</t>
+  </si>
+  <si>
+    <t>X97_reg3</t>
+  </si>
+  <si>
+    <t>X99_1225A</t>
+  </si>
+  <si>
+    <t>X99_1225B</t>
+  </si>
+  <si>
+    <t>X99_8741C</t>
+  </si>
+  <si>
+    <t>X99_8741D</t>
+  </si>
+  <si>
+    <t>X36_5459A__x5459B_M_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X36_5459B__x5459C_M_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X36_8667C__x8667B_F_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X86_reg1__x6197B_M_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X86_reg2__x5993B_F_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X86_reg3__x5993C_F_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X97_reg1__x1735B_M_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X97_reg2__x1735C_M_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X97_reg3__x6588C_F_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X99_1225A__x1225B_M_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X99_1225B__x1225C_M_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X99_8741C__x8741C_F_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X99_8741D__x8741D_F_domainbounds.tiff</t>
   </si>
 </sst>
 </file>
@@ -1079,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6A2C30-26A8-B54C-BC2B-4A3CBE89BCC7}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1091,7 +1133,7 @@
     <col min="8" max="8" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1117,10 +1159,13 @@
         <v>32</v>
       </c>
       <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1143,13 +1188,16 @@
         <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1172,13 +1220,16 @@
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1201,13 +1252,16 @@
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>55</v>
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1230,13 +1284,16 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1259,13 +1316,16 @@
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1288,13 +1348,16 @@
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>49</v>
+        <v>36</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1317,13 +1380,16 @@
         <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1346,13 +1412,16 @@
         <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1375,13 +1444,16 @@
         <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1404,13 +1476,16 @@
         <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>43</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1433,13 +1508,16 @@
         <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>44</v>
+      </c>
+      <c r="J12" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1462,13 +1540,16 @@
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>45</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1491,10 +1572,13 @@
         <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>46</v>
+      </c>
+      <c r="J14" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated samui to include flipped coordinate matrices and conversion from R object to .h5 object
</commit_message>
<xml_diff>
--- a/xenium_HYP/raw-data/sample-info/demos_by_sampleid-xen.xlsx
+++ b/xenium_HYP/raw-data/sample-info/demos_by_sampleid-xen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/zk/dyx0glj52sn6_7db_dn0p2vc0000gn/T/ch.sudo.cyberduck/editor-3f24765b-cc4f-4bd7-8256-e435931ba961/dcs04/lieber/marmaypag/spatialHYP_LIBD4195/spatial_HYP/xenium_HYP/raw-data/sample-info/528783301/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/zk/dyx0glj52sn6_7db_dn0p2vc0000gn/T/fz3temp-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8FBC81-1BC6-7C40-A1F0-07DE79332841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397A4191-63A8-764C-B626-405979607408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3440" windowWidth="24440" windowHeight="12940" xr2:uid="{1DB9EFC4-81BF-1747-9C05-D3C9C2D83113}"/>
   </bookViews>
@@ -218,9 +218,6 @@
     <t>X99_8741D</t>
   </si>
   <si>
-    <t>X36_5459A__x5459B_M_domainbounds.tiff</t>
-  </si>
-  <si>
     <t>X36_5459B__x5459C_M_domainbounds.tiff</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>X99_8741D__x8741D_F_domainbounds.tiff</t>
+  </si>
+  <si>
+    <t>X36_5459A_domainbounds_3chantiftest.tiff</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1124,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1188,7 +1188,7 @@
         <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
         <v>40</v>
@@ -1220,7 +1220,7 @@
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I3" t="s">
         <v>41</v>
@@ -1252,7 +1252,7 @@
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I4" t="s">
         <v>42</v>
@@ -1284,7 +1284,7 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
         <v>33</v>
@@ -1316,7 +1316,7 @@
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I6" t="s">
         <v>35</v>
@@ -1348,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I7" t="s">
         <v>36</v>
@@ -1380,7 +1380,7 @@
         <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
         <v>37</v>
@@ -1412,7 +1412,7 @@
         <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
         <v>38</v>
@@ -1444,7 +1444,7 @@
         <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
         <v>39</v>
@@ -1476,7 +1476,7 @@
         <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I11" t="s">
         <v>43</v>
@@ -1508,7 +1508,7 @@
         <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I12" t="s">
         <v>44</v>
@@ -1540,7 +1540,7 @@
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I13" t="s">
         <v>45</v>
@@ -1572,7 +1572,7 @@
         <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I14" t="s">
         <v>46</v>

</xml_diff>